<commit_message>
Changed from localhost to heroku
</commit_message>
<xml_diff>
--- a/Design_db_sys.xlsx
+++ b/Design_db_sys.xlsx
@@ -361,7 +361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>XYZ789</t>
   </si>
@@ -717,9 +717,6 @@
     <t>0-a2</t>
   </si>
   <si>
-    <t>Corresponding DC values are auto-fetched &amp; stored from Ref API, on saving Installation Metadata</t>
-  </si>
-  <si>
     <t>0-b</t>
   </si>
   <si>
@@ -884,6 +881,15 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Corresponding Ref DC values are auto-fetched &amp; stored from Ref API, on saving Installation Metadata</t>
+  </si>
+  <si>
+    <t>Manual (currently)</t>
+  </si>
+  <si>
+    <t>Manual/scheduled</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1045,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1408,26 +1414,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1452,8 +1443,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1464,110 +1455,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1575,84 +1467,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1665,12 +1496,176 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2641,7 +2636,7 @@
   <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2702,17 +2697,17 @@
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="64"/>
-      <c r="C10" s="66" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -2721,7 +2716,7 @@
       <c r="E10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="20" t="s">
@@ -2744,7 +2739,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="65"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="10" t="s">
         <v>3</v>
       </c>
@@ -2779,8 +2774,8 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
-      <c r="C12" s="67" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="11">
@@ -2814,8 +2809,8 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="65"/>
-      <c r="C13" s="67" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="34" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="11">
@@ -2849,7 +2844,7 @@
       </c>
     </row>
     <row r="14" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="65"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="10" t="s">
         <v>0</v>
       </c>
@@ -2875,20 +2870,20 @@
     </row>
     <row r="15" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11"/>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="I15" s="33" t="s">
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
+      <c r="I15" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="35"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="54"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G16" s="11"/>
@@ -2948,74 +2943,74 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="27"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="46"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="59"/>
     </row>
     <row r="3" spans="2:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-      <c r="D3" s="69" t="s">
+      <c r="B3" s="93"/>
+      <c r="D3" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71"/>
-      <c r="H3" s="81" t="s">
+      <c r="E3" s="65"/>
+      <c r="F3" s="66"/>
+      <c r="H3" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="82" t="s">
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="85"/>
-      <c r="O3" s="76"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="36"/>
     </row>
     <row r="4" spans="2:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="40"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="74"/>
-      <c r="H4" s="87" t="s">
+      <c r="B4" s="93"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="H4" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="79" t="s">
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="79"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="80"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="78"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="93"/>
     </row>
     <row r="6" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="40"/>
+      <c r="B6" s="93"/>
     </row>
     <row r="7" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="40"/>
-      <c r="D7" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="52"/>
+      <c r="B7" s="93"/>
+      <c r="D7" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="82"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -3026,21 +3021,21 @@
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="40"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="54"/>
+      <c r="B8" s="93"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="84"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="57" t="s">
+      <c r="H8" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="58"/>
+      <c r="I8" s="87"/>
       <c r="J8" s="11"/>
       <c r="N8" s="12"/>
     </row>
     <row r="9" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="40"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56"/>
+      <c r="B9" s="93"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="86"/>
       <c r="G9" s="10"/>
       <c r="H9" s="28"/>
       <c r="I9" s="24"/>
@@ -3051,25 +3046,25 @@
       <c r="N9" s="12"/>
     </row>
     <row r="10" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="40"/>
-      <c r="D10" s="44" t="s">
+      <c r="B10" s="93"/>
+      <c r="D10" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="46"/>
+      <c r="E10" s="59"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="86"/>
-      <c r="J10" s="77"/>
-      <c r="L10" s="57" t="s">
+      <c r="I10" s="80"/>
+      <c r="J10" s="81"/>
+      <c r="L10" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="77"/>
+      <c r="M10" s="81"/>
       <c r="N10" s="12"/>
     </row>
     <row r="11" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
+      <c r="B11" s="93"/>
       <c r="G11" s="10"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -3080,70 +3075,77 @@
       <c r="N11" s="12"/>
     </row>
     <row r="12" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="41"/>
-      <c r="G12" s="44" t="s">
+      <c r="B12" s="94"/>
+      <c r="G12" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="46"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="59"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="51"/>
-      <c r="L15" s="47" t="s">
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="62"/>
+      <c r="L15" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="48"/>
+      <c r="M15" s="98"/>
     </row>
     <row r="16" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="37"/>
-      <c r="G16" s="44" t="s">
+      <c r="B16" s="90"/>
+      <c r="G16" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="46"/>
-      <c r="L16" s="44" t="s">
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="59"/>
+      <c r="L16" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="46"/>
+      <c r="M16" s="59"/>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="37"/>
+      <c r="B17" s="90"/>
     </row>
     <row r="18" spans="2:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="37"/>
-      <c r="L18" s="69" t="s">
+      <c r="B18" s="90"/>
+      <c r="L18" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="M18" s="42"/>
-      <c r="N18" s="43"/>
+      <c r="M18" s="95"/>
+      <c r="N18" s="96"/>
     </row>
     <row r="19" spans="2:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="38"/>
-      <c r="L19" s="44" t="s">
+      <c r="B19" s="91"/>
+      <c r="L19" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="M19" s="45"/>
-      <c r="N19" s="46"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="59"/>
     </row>
     <row r="20" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="G16:J16"/>
@@ -3160,13 +3162,6 @@
     <mergeCell ref="D7:E9"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="L10:M10"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3180,16 +3175,16 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="6"/>
     <col min="2" max="2" width="12.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="85.625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11" style="6"/>
+    <col min="5" max="5" width="15.5" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="6"/>
     <col min="8" max="8" width="39.625" style="6" bestFit="1" customWidth="1"/>
@@ -3201,133 +3196,137 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="98" t="s">
+    <row r="3" spans="2:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="101" t="s">
+      <c r="D3" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="102" t="s">
+    </row>
+    <row r="5" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="105" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="93" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="94" t="s">
+      <c r="E5" s="49"/>
+    </row>
+    <row r="6" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="106" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="37">
+        <v>2</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="50"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="37">
+        <v>3</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="50"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="37">
+        <v>4</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="50"/>
+    </row>
+    <row r="12" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="107" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="43">
+        <v>5</v>
+      </c>
+      <c r="D12" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="103" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="94" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="103"/>
-    </row>
-    <row r="6" spans="2:5" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="93" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="103" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="93" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="103"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="78">
-        <v>1</v>
-      </c>
-      <c r="D8" s="92" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="103" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="78">
-        <v>2</v>
-      </c>
-      <c r="D9" s="94" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="104"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="95" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="78">
-        <v>3</v>
-      </c>
-      <c r="D10" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="104"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="95" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="78">
-        <v>4</v>
-      </c>
-      <c r="D11" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="104"/>
-    </row>
-    <row r="12" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="96" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="97">
-        <v>5</v>
-      </c>
-      <c r="D12" s="105" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="106"/>
+      <c r="E12" s="106" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3374,44 +3373,44 @@
       </c>
       <c r="G5" s="1"/>
       <c r="L5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M5" s="1"/>
       <c r="P5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="N7" s="59" t="s">
+      <c r="E7" s="100"/>
+      <c r="N7" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="60"/>
+      <c r="O7" s="100"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D8" s="90" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="91"/>
-      <c r="N8" s="90" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="91"/>
+      <c r="D8" s="103" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="104"/>
+      <c r="N8" s="103" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="104"/>
     </row>
     <row r="9" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="N9" s="61" t="s">
+      <c r="E9" s="102"/>
+      <c r="N9" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="62"/>
+      <c r="O9" s="102"/>
     </row>
     <row r="10" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
@@ -3442,11 +3441,11 @@
       </c>
       <c r="G12" s="1"/>
       <c r="L12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M12" s="1"/>
       <c r="P12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q12" s="1"/>
     </row>

</xml_diff>